<commit_message>
Update ChIP-seq analysis documentation
</commit_message>
<xml_diff>
--- a/nanni_chip_rna_2022/documentation/chipSeq_analysis_pipeline_04avn.xlsx
+++ b/nanni_chip_rna_2022/documentation/chipSeq_analysis_pipeline_04avn.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SHARE\McIntyre_Lab\Dros_CHIP_RNA_ms\documentation\ChIP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SHARE\McIntyre_Lab\Dros_CHIP_RNA_ms\documentation\github_documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386EE71B-5850-4ABD-889C-294480A31E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A7E15B-29E1-4C98-8FFF-7F2B5E14368C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8808" yWindow="3144" windowWidth="15672" windowHeight="8568" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="15672" windowHeight="9924" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall ChIP-seq Analysis" sheetId="1" r:id="rId1"/>
@@ -103,18 +103,6 @@
     <t>run_cut_bbM_fqSplit_chipSeq_04avn.sbatch</t>
   </si>
   <si>
-    <t>(1) Remove adapter sequences with cutadapt
-(2) Merge R1-R2 with bbmerge, min overlap of 25% the original read length and remove merged reads that are less than 50% original read length plus 14
-(3) Split out reads &lt; 50% original read length and remove empty pairs generated by cutadapt
-(3) Run fqSplitDups on
-    Bbmerge (PE)
-    Widow R1 (SE)
-    Widow R2 (SE)
-    Unmerge (no empty) R1 (SE)
-    Unmerge (no empty) R2 (SE)
-** Intermediate files are removed after they are used within the script – only keep fqSplitDups output files in the end</t>
-  </si>
-  <si>
     <t>cutadapt/2.1 
 bbmap/38.44
 (python/2.7.14) $PROJ/scripts/chipseq/bbM_50perc_readLen_and_drop_empty_reads_05amm.py
@@ -128,10 +116,6 @@
   </si>
   <si>
     <t>Call peaks with MACS2</t>
-  </si>
-  <si>
-    <t>Generate a temporary design file of all non-input samples
-Loop through samples to call peaks with MACS2 using the corresponding input sample</t>
   </si>
   <si>
     <t>Combine replicate peaks</t>
@@ -732,6 +716,23 @@
 module load R/3.6
 $PROJ/scripts/venn_diagram.py
 $PROJ/scripts/venn_diagram.R</t>
+  </si>
+  <si>
+    <t>(1) Remove adapter sequences with cutadapt
+(2) Merge R1-R2 with bbmerge, min overlap of 25% the original read length and remove merged reads that are less than 50% original read length plus 14
+(3) Split out reads &lt; 50% original read length and remove empty pairs generated by cutadapt
+(3) Run fqSplitDups on
+    Bbmerge (SE)
+    Widow R1 (SE)
+    Widow R2 (SE)
+    Unmerge (no empty) R1 (PE)
+    Unmerge (no empty) R2 (PE)
+** Intermediate files are removed after they are used within the script – only keep fqSplitDups output files in the end</t>
+  </si>
+  <si>
+    <t>Generate a temporary design file of all non-input samples
+Loop through samples to call peaks with MACS2 using the corresponding input sample
+** Use --nomodel --shift 73 --extsize 143 based on size of nucleosome footprint and description of how these arguments work in MACS2 documentation (https://github.com/macs3-project/MACS/blob/master/docs/callpeak.md#--nomodel)</t>
   </si>
 </sst>
 </file>
@@ -1290,7 +1291,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1307,7 +1310,7 @@
     <row r="1" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -1453,13 +1456,13 @@
         <v>15</v>
       </c>
       <c r="E10" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="F10" s="16" t="s">
-        <v>79</v>
-      </c>
       <c r="G10" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H10" s="16"/>
     </row>
@@ -1481,22 +1484,22 @@
         <v>16</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="23" t="s">
         <v>68</v>
-      </c>
-      <c r="G12" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="H12" s="23" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:1024" x14ac:dyDescent="0.25">
@@ -1520,19 +1523,19 @@
         <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F14" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" s="24" t="s">
         <v>71</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:1024" x14ac:dyDescent="0.25">
@@ -1550,7 +1553,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>20</v>
@@ -1559,10 +1562,10 @@
         <v>21</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H16" s="26"/>
       <c r="AMJ16" s="3"/>
@@ -1587,7 +1590,7 @@
         <v>22</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>20</v>
@@ -1596,10 +1599,10 @@
         <v>23</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="8"/>
@@ -1693,7 +1696,7 @@
   <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1710,7 +1713,7 @@
     <row r="1" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
       <c r="B1" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
@@ -1838,30 +1841,30 @@
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
     </row>
-    <row r="10" spans="1:21" ht="145.19999999999999" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="198" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>30</v>
+        <v>126</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>21</v>
       </c>
       <c r="E10" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="16" t="s">
         <v>80</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -1875,25 +1878,25 @@
         <v>12</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>21</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -1908,25 +1911,25 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D14" s="16" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -1941,25 +1944,25 @@
         <v>12</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1979,25 +1982,25 @@
         <v>12</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -2016,25 +2019,25 @@
         <v>12</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D20" s="16" t="s">
         <v>21</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H20" s="28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2045,22 +2048,22 @@
         <v>12</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D22" s="16" t="s">
         <v>21</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2085,7 +2088,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CF9A06-6C26-4DC5-A368-CAEADAE909C7}">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2101,7 +2106,7 @@
     <row r="1" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
       <c r="B1" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
@@ -2234,22 +2239,22 @@
         <v>12</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -2267,22 +2272,22 @@
         <v>12</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -2293,25 +2298,25 @@
         <v>12</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E14" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="F14" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>110</v>
-      </c>
       <c r="H14" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="237.6" x14ac:dyDescent="0.25">
@@ -2319,25 +2324,25 @@
         <v>12</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2357,25 +2362,25 @@
         <v>12</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -2394,22 +2399,22 @@
         <v>12</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C20" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D20" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="16" t="s">
+      <c r="G20" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="8"/>
@@ -2429,25 +2434,25 @@
         <v>12</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E22" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="F22" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="F22" s="16" t="s">
-        <v>123</v>
-      </c>
       <c r="G22" s="16" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="118.8" x14ac:dyDescent="0.25">
@@ -2455,25 +2460,25 @@
         <v>12</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update documentation, scripts, and analysis output directories
</commit_message>
<xml_diff>
--- a/nanni_chip_rna_2022/documentation/chipSeq_analysis_pipeline_04avn.xlsx
+++ b/nanni_chip_rna_2022/documentation/chipSeq_analysis_pipeline_04avn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SHARE\McIntyre_Lab\Dros_CHIP_RNA_ms\documentation\github_documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ufgi$/SHARE/McIntyre_Lab/Dros_CHIP_RNA_ms/documentation/github_documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A7E15B-29E1-4C98-8FFF-7F2B5E14368C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB403A1-EE73-574B-9C0A-F915138A212D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="15672" windowHeight="9924" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1120" yWindow="1120" windowWidth="21080" windowHeight="14840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall ChIP-seq Analysis" sheetId="1" r:id="rId1"/>
@@ -680,13 +680,6 @@
 $SCRIPTS/merge_GO_ID.py</t>
   </si>
   <si>
-    <t>/ufrc/mcintyre/share/references/dsim_fb202/gene2go_with_terms_from_mel_ortho.csv
-$PROJ/chipseq/detection_above_background/features/
-${SPECIES}_chip_features*
-${SPECIES}_DAI_gene_lists*
-${SPECIES}_chip_features*</t>
-  </si>
-  <si>
     <t>/ufrc/mcintyre/share/references/dmel_fb617/gene2go_with_terms_02jrbn.csv
 /ufrc/mcintyre/share/etoh_srna/ortholog_files/dmel_orthologs_dsim_fb_2017_04.csv
 /ufrc/mcintyre/share/references/dmel_fb617/dmel617_annotations_100bp_reads/deml617_100bp_exon_fragments_coverage.bed
@@ -733,6 +726,15 @@
     <t>Generate a temporary design file of all non-input samples
 Loop through samples to call peaks with MACS2 using the corresponding input sample
 ** Use --nomodel --shift 73 --extsize 143 based on size of nucleosome footprint and description of how these arguments work in MACS2 documentation (https://github.com/macs3-project/MACS/blob/master/docs/callpeak.md#--nomodel)</t>
+  </si>
+  <si>
+    <t>/ufrc/mcintyre/share/references/dsim_fb202/gene2go_with_terms_from_mel_ortho.csv
+$PROJ/chipseq/detection_above_background/features/
+${SPECIES}_chip_features*
+${SPECIES}_DAI_gene_lists*
+${SPECIES}_chip_features*
+${SPECIES}_chip_5U_3U_TSS_frag_intr_inter_flag.csv
+${SPECIES}_chip_5U_3U_TSS_fus_intr_inter_flag.csv</t>
   </si>
 </sst>
 </file>
@@ -1291,23 +1293,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="1"/>
-    <col min="2" max="2" width="24.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="1"/>
+    <col min="2" max="2" width="24.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="30.6640625" style="2" customWidth="1"/>
-    <col min="4" max="5" width="30.5546875" style="2" customWidth="1"/>
+    <col min="4" max="5" width="30.5" style="2" customWidth="1"/>
     <col min="6" max="7" width="35" style="2" customWidth="1"/>
     <col min="8" max="8" width="30" style="2" customWidth="1"/>
-    <col min="9" max="1023" width="11.5546875" style="3"/>
+    <col min="9" max="1023" width="11.5" style="3"/>
     <col min="1024" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1024" s="7" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="2"/>
       <c r="B1" s="4" t="s">
         <v>27</v>
@@ -1321,7 +1323,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1024" s="7" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -1335,7 +1337,7 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
       <c r="B3" s="4"/>
       <c r="C3" s="2"/>
@@ -1347,7 +1349,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:1024" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1024" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="2"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
@@ -1359,7 +1361,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1024" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="2"/>
       <c r="B5" s="4"/>
       <c r="C5" s="2" t="s">
@@ -1369,14 +1371,14 @@
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A6" s="2"/>
       <c r="B6" s="4"/>
       <c r="H6" s="5"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
       <c r="H7" s="5"/>
       <c r="I7" s="8"/>
@@ -1393,7 +1395,7 @@
       <c r="T7" s="9"/>
       <c r="U7" s="9"/>
     </row>
-    <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1024" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="10" t="s">
         <v>4</v>
       </c>
@@ -1432,7 +1434,7 @@
       <c r="T8" s="14"/>
       <c r="U8" s="14"/>
     </row>
-    <row r="9" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A9" s="15"/>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
@@ -1442,7 +1444,7 @@
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
     </row>
-    <row r="10" spans="1:1024" ht="66" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1024" ht="70" x14ac:dyDescent="0.15">
       <c r="A10" s="15" t="s">
         <v>12</v>
       </c>
@@ -1466,7 +1468,7 @@
       </c>
       <c r="H10" s="16"/>
     </row>
-    <row r="11" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
@@ -1476,7 +1478,7 @@
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
     </row>
-    <row r="12" spans="1:1024" ht="316.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1024" ht="332" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
@@ -1484,7 +1486,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>24</v>
@@ -1502,7 +1504,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
@@ -1512,7 +1514,7 @@
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
     </row>
-    <row r="14" spans="1:1024" ht="316.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1024" ht="293" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1538,14 +1540,14 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="B15" s="5"/>
       <c r="D15" s="18"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:1024" ht="66" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1024" ht="70" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1570,7 +1572,7 @@
       <c r="H16" s="26"/>
       <c r="AMJ16" s="3"/>
     </row>
-    <row r="17" spans="1:1024" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1024" s="9" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="2"/>
@@ -1582,7 +1584,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:1024" ht="66" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1024" ht="70" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
@@ -1609,7 +1611,7 @@
       <c r="J18" s="8"/>
       <c r="AMJ18" s="3"/>
     </row>
-    <row r="19" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="F19" s="5"/>
@@ -1619,66 +1621,66 @@
       <c r="J19" s="8"/>
       <c r="AMJ19" s="3"/>
     </row>
-    <row r="20" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="AMJ20" s="3"/>
     </row>
-    <row r="21" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="C21" s="4"/>
       <c r="AMJ21" s="3"/>
     </row>
-    <row r="22" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="AMJ22" s="3"/>
     </row>
-    <row r="23" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="AMJ23" s="3"/>
     </row>
-    <row r="24" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="AMJ24" s="3"/>
     </row>
-    <row r="25" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="AMJ25" s="3"/>
     </row>
-    <row r="26" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="AMJ26" s="3"/>
     </row>
-    <row r="27" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="AMJ27" s="3"/>
     </row>
-    <row r="28" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="B28" s="5"/>
       <c r="F28" s="5"/>
       <c r="H28" s="5"/>
       <c r="AMJ28" s="3"/>
     </row>
-    <row r="29" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="AMJ29" s="3"/>
     </row>
-    <row r="30" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="H30" s="5"/>
       <c r="AMJ30" s="3"/>
     </row>
-    <row r="42" spans="1024:1024" x14ac:dyDescent="0.25">
+    <row r="42" spans="1024:1024" x14ac:dyDescent="0.15">
       <c r="AMJ42" s="3"/>
     </row>
-    <row r="43" spans="1024:1024" x14ac:dyDescent="0.25">
+    <row r="43" spans="1024:1024" x14ac:dyDescent="0.15">
       <c r="AMJ43" s="3"/>
     </row>
-    <row r="44" spans="1024:1024" x14ac:dyDescent="0.25">
+    <row r="44" spans="1024:1024" x14ac:dyDescent="0.15">
       <c r="AMJ44" s="3"/>
     </row>
-    <row r="45" spans="1024:1024" x14ac:dyDescent="0.25">
+    <row r="45" spans="1024:1024" x14ac:dyDescent="0.15">
       <c r="AMJ45" s="3"/>
     </row>
-    <row r="46" spans="1024:1024" x14ac:dyDescent="0.25">
+    <row r="46" spans="1024:1024" x14ac:dyDescent="0.15">
       <c r="AMJ46" s="3"/>
     </row>
-    <row r="47" spans="1024:1024" x14ac:dyDescent="0.25">
+    <row r="47" spans="1024:1024" x14ac:dyDescent="0.15">
       <c r="AMJ47" s="3"/>
     </row>
-    <row r="48" spans="1024:1024" x14ac:dyDescent="0.25">
+    <row r="48" spans="1024:1024" x14ac:dyDescent="0.15">
       <c r="AMJ48" s="3"/>
     </row>
-    <row r="49" spans="1024:1024" x14ac:dyDescent="0.25">
+    <row r="49" spans="1024:1024" x14ac:dyDescent="0.15">
       <c r="AMJ49" s="3"/>
     </row>
   </sheetData>
@@ -1695,22 +1697,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E966CA05-E937-4CA5-8B44-5CB3A0A056FD}">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="15"/>
-    <col min="2" max="2" width="24.77734375" style="16" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="15"/>
+    <col min="2" max="2" width="24.83203125" style="16" customWidth="1"/>
     <col min="3" max="3" width="30.6640625" style="16" customWidth="1"/>
-    <col min="4" max="5" width="30.5546875" style="16" customWidth="1"/>
+    <col min="4" max="5" width="30.5" style="16" customWidth="1"/>
     <col min="6" max="7" width="35" style="16" customWidth="1"/>
     <col min="8" max="8" width="30" style="16" customWidth="1"/>
     <col min="1024" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="19" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="16"/>
       <c r="B1" s="4" t="s">
         <v>41</v>
@@ -1724,7 +1726,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="19" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="16"/>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -1738,7 +1740,7 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="16"/>
       <c r="B3" s="4"/>
       <c r="C3" s="16"/>
@@ -1750,7 +1752,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="16"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
@@ -1762,7 +1764,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="16"/>
       <c r="B5" s="4"/>
       <c r="C5" s="16" t="s">
@@ -1772,14 +1774,14 @@
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A6" s="16"/>
       <c r="B6" s="4"/>
       <c r="H6" s="5"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A7" s="16"/>
       <c r="H7" s="5"/>
       <c r="I7" s="8"/>
@@ -1796,7 +1798,7 @@
       <c r="T7" s="20"/>
       <c r="U7" s="20"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="10" t="s">
         <v>4</v>
       </c>
@@ -1835,13 +1837,13 @@
       <c r="T8" s="14"/>
       <c r="U8" s="14"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
     </row>
-    <row r="10" spans="1:21" ht="198" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="210" x14ac:dyDescent="0.15">
       <c r="A10" s="15" t="s">
         <v>12</v>
       </c>
@@ -1849,7 +1851,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>21</v>
@@ -1867,13 +1869,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" spans="1:21" ht="118.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="126" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
@@ -1899,14 +1901,14 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
       <c r="D13" s="18"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:21" ht="396" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="358" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
         <v>12</v>
       </c>
@@ -1932,14 +1934,14 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B15" s="5"/>
       <c r="D15" s="18"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:21" ht="184.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="196" x14ac:dyDescent="0.15">
       <c r="A16" s="15" t="s">
         <v>12</v>
       </c>
@@ -1965,7 +1967,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="16"/>
@@ -1977,7 +1979,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="200.4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="198" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
@@ -2005,7 +2007,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="F19" s="5"/>
@@ -2014,7 +2016,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="145.19999999999999" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="140" x14ac:dyDescent="0.15">
       <c r="A20" s="15" t="s">
         <v>12</v>
       </c>
@@ -2040,10 +2042,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:10" ht="105.6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="98" x14ac:dyDescent="0.15">
       <c r="A22" s="15" t="s">
         <v>12</v>
       </c>
@@ -2066,12 +2068,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B28" s="5"/>
       <c r="F28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
       <c r="H30" s="5"/>
     </row>
   </sheetData>
@@ -2088,22 +2090,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CF9A06-6C26-4DC5-A368-CAEADAE909C7}">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="15"/>
-    <col min="2" max="2" width="24.77734375" style="16" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="15"/>
+    <col min="2" max="2" width="24.83203125" style="16" customWidth="1"/>
     <col min="3" max="3" width="30.6640625" style="16" customWidth="1"/>
-    <col min="4" max="5" width="30.5546875" style="16" customWidth="1"/>
+    <col min="4" max="5" width="30.5" style="16" customWidth="1"/>
     <col min="6" max="7" width="35" style="16" customWidth="1"/>
     <col min="8" max="8" width="30" style="16" customWidth="1"/>
     <col min="1024" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="19" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="16"/>
       <c r="B1" s="4" t="s">
         <v>57</v>
@@ -2117,7 +2119,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="19" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="16"/>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -2131,7 +2133,7 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="16"/>
       <c r="B3" s="4"/>
       <c r="C3" s="16"/>
@@ -2143,7 +2145,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="16"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
@@ -2155,7 +2157,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="16"/>
       <c r="B5" s="4"/>
       <c r="C5" s="16" t="s">
@@ -2165,14 +2167,14 @@
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A6" s="16"/>
       <c r="B6" s="4"/>
       <c r="H6" s="5"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A7" s="16"/>
       <c r="H7" s="5"/>
       <c r="I7" s="8"/>
@@ -2189,7 +2191,7 @@
       <c r="T7" s="20"/>
       <c r="U7" s="20"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="10" t="s">
         <v>4</v>
       </c>
@@ -2228,13 +2230,13 @@
       <c r="T8" s="14"/>
       <c r="U8" s="14"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
     </row>
-    <row r="10" spans="1:21" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A10" s="15" t="s">
         <v>12</v>
       </c>
@@ -2257,7 +2259,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" s="25" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A11" s="15"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -2267,7 +2269,7 @@
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
     </row>
-    <row r="12" spans="1:21" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
@@ -2290,10 +2292,10 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:21" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="56" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
         <v>12</v>
       </c>
@@ -2319,7 +2321,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="237.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="252" x14ac:dyDescent="0.15">
       <c r="A16" s="15" t="s">
         <v>12</v>
       </c>
@@ -2345,7 +2347,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="16"/>
@@ -2357,7 +2359,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="198" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="210" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
@@ -2385,7 +2387,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="F19" s="5"/>
@@ -2394,7 +2396,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
         <v>12</v>
       </c>
@@ -2420,7 +2422,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="F21" s="5"/>
@@ -2429,7 +2431,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A22" s="15" t="s">
         <v>12</v>
       </c>
@@ -2446,16 +2448,16 @@
         <v>119</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="H22" s="16" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="118.8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="126" x14ac:dyDescent="0.15">
       <c r="A24" s="15" t="s">
         <v>12</v>
       </c>
@@ -2469,24 +2471,24 @@
         <v>60</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F24" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="G24" s="16" t="s">
         <v>122</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>123</v>
       </c>
       <c r="H24" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B26" s="5"/>
       <c r="F26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
       <c r="H28" s="5"/>
     </row>
   </sheetData>

</xml_diff>